<commit_message>
finished all harmonisation rules for respective variables
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_DEGS1_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_DEGS1_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{E97C809B-3102-435E-9A58-D3EF5F875857}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{8EA9B79E-A9F2-4569-BCFF-40137F6F402C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="373">
   <si>
     <t>index</t>
   </si>
@@ -899,13 +899,375 @@
   </si>
   <si>
     <t>Wie oft und wieviel Nudeln und Reis</t>
+  </si>
+  <si>
+    <t>FQvbrot1;FQvbrot2;FQmbrot1;FQmbrot2;FQwbrot1;FQwbrot2</t>
+  </si>
+  <si>
+    <t>(FQvbrot1*FQvbrot2)+(FQmbrot1*FQmbrot2)+(FQwbrot1*FQwbrot2)</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Vollkornbrot oder -brötchen, Grau- oder Mischbrot, Weißbrot oder Brötchen</t>
+  </si>
+  <si>
+    <t>FQcorn1;FQcorn2;FQmuesli1;FQmuesli2</t>
+  </si>
+  <si>
+    <t>(FQcorn1*FQcorn2)+(FQmuesli1*FQmuesli2)</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Cornflakes und Müsli</t>
+  </si>
+  <si>
+    <t>FQcrack1;FQcrack2</t>
+  </si>
+  <si>
+    <t>FQcrack1*FQcrack2</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Salzgebäck und Cracker</t>
+  </si>
+  <si>
+    <t>FQfleisch1*FQfleisch2</t>
+  </si>
+  <si>
+    <t>FQfleisch1;FQfleisch2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie oft und wieviel Fleisch (ohne Geflügel, ohne Wurst) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Was machen wir mit FQfleisch3 (Wie oft paniertes Flesich)?</t>
+    </r>
+  </si>
+  <si>
+    <t>FQhuhn1;FQhuhn2</t>
+  </si>
+  <si>
+    <t>FQhuhn1*FQhuhn2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie oft und wieviel Geflügel
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Was machen wir mit FGhuhn3 (Anteil paniertes o frittiertes Geflügel)?</t>
+    </r>
+  </si>
+  <si>
+    <t>(FQburg1*FQburg2)+(FQcwurst1*FQcwurst2)+(FQwurst1*FQwurst2)+(FQschink1*FQschink2)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie oft und wieviel Hamburger oder Döner Kebab? Wie oft und wiviel Brat- oder Currywurst? Wie oft und wieivel Wurst? Wie oft und wieviel Schinken? 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Was machen wir mit FQwurst3 (Wie oft fettarme Wurst)?</t>
+    </r>
+  </si>
+  <si>
+    <t>FQburg1;FQburg2;FQcwurst1;FQcwurst2;FQwurst1;FQwurst2;FQschink1;FQschink2</t>
+  </si>
+  <si>
+    <t>FQkfisch1;FQkfisch2;FQwfisch1;FQwfisch2</t>
+  </si>
+  <si>
+    <t>(FQkfisch1*FQkfisch2)+(FQwfisch1*FQwfisch2)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie oft und wieviel kalter Fisch? Wie oft und wieviel warmer Fisch?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Was machen wir mit FQwfisch3 (Anteil panierter Fisch)?</t>
+    </r>
+  </si>
+  <si>
+    <t>FQei1;FQei2</t>
+  </si>
+  <si>
+    <t>FQei1*FQei2</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Eier?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complete </t>
+  </si>
+  <si>
+    <t>FQsfett1;FQsfett2</t>
+  </si>
+  <si>
+    <t>FQsfett1*FQsfett2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie oft und wieviel Butter oder Margarine?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Achtung: keine pflanzl. Öle!</t>
+    </r>
+  </si>
+  <si>
+    <t>FQhonig1;FQhonig2;FQncreme1;FQncreme2</t>
+  </si>
+  <si>
+    <t>Wie of und wieviel Honig oder Marmelade? Wie oft und wieviel Nuss-Nougatcreme?</t>
+  </si>
+  <si>
+    <t>FQschok1;FQschok2</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Schokolade oder Schokeriegel?</t>
+  </si>
+  <si>
+    <t>FQsuess1;FQsuess2</t>
+  </si>
+  <si>
+    <t>FQsuess1*FQsuess2</t>
+  </si>
+  <si>
+    <t>FQschok1*FQschok2</t>
+  </si>
+  <si>
+    <t>(FQhonig1*FQhonig2)+(FQncreme1*FQncreme2)</t>
+  </si>
+  <si>
+    <t>FQeis1;FQeis2</t>
+  </si>
+  <si>
+    <t>FQeis1*FQeis2</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Eis?</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Süßigkeiten?</t>
+  </si>
+  <si>
+    <t>FQkuch1;FQkuch2;FQkeks1;FQkeks2</t>
+  </si>
+  <si>
+    <t>(FQkuch1*FQkuch2)+(FQkeks1*FQkeks2)</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Kuchen, Torten oder süße Backwaren?
+Wie oft und wieviel Kekse?</t>
+  </si>
+  <si>
+    <t>FQfsaft1;FQfsaft2;FQgsaft1;FQgsaft2</t>
+  </si>
+  <si>
+    <t>(FQfsaft1*FQfsaft2)+(FQgsaft1*FQgsaft2)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie oft und wieviel Fruchtsaft?
+Wie oft und wieviel Gemüsesaft?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Was machen wir mit FGfsaft3 (Fruchtsaftverdünnt/unverdünnt)? 
+Was machen wir mit FQgsaft3 (Gemüsesaft verdünnt/unverdünnt)?</t>
+    </r>
+  </si>
+  <si>
+    <t>FQcola1;FQcola2;FQlight1;FQlight2</t>
+  </si>
+  <si>
+    <t>(FQcola1*FQcola2)+(FQlight1*FQlight2)</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel zuckerh. Erfrischungsgetränke?
+Wie oft und wieviel kal.red. Erfrischungsgetränke?</t>
+  </si>
+  <si>
+    <t>FQkaff1;FQkaff2</t>
+  </si>
+  <si>
+    <t>FQkaff1*FQkaff2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie oft und wieviel Kaffee?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Was machen wir mit FQkaff3 (Zucker: Kaffee)?</t>
+    </r>
+  </si>
+  <si>
+    <t>FQstee1;FQstee2</t>
+  </si>
+  <si>
+    <t>FQstee1*FQstee2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie oft und wieviel schwarzer oder grüner Tee?
+Was machen wir mit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FQstee3 (Zucker:Schwarzer oder grüner Tee)?</t>
+    </r>
+  </si>
+  <si>
+    <t>FQftee1;FQftee2</t>
+  </si>
+  <si>
+    <t>FQftee1*FQftee2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie oft und wieviel Früchte- oder Kräutertee?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Was machen wir mit FQftee3 (Zucker: Früchte- oder Kräutertee)?</t>
+    </r>
+  </si>
+  <si>
+    <t>FQwass1;FQwass2</t>
+  </si>
+  <si>
+    <t>FQwass1*FQwass2</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Wasser?</t>
+  </si>
+  <si>
+    <t>FQwein1;FQwein2</t>
+  </si>
+  <si>
+    <t>FQwein1*FQwein2</t>
+  </si>
+  <si>
+    <t>Wie oft  und wieviel Wein, Sekt, Obstwein?</t>
+  </si>
+  <si>
+    <t>FQbier1;FQbier2</t>
+  </si>
+  <si>
+    <t>FQbier1*FQbier2</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Bier?</t>
+  </si>
+  <si>
+    <t>FQschnaps1;FQschnaps2</t>
+  </si>
+  <si>
+    <t>FQschnaps1*FQschnaps2</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel hochprozentige alkoholische Getränke?</t>
+  </si>
+  <si>
+    <t>FQcockt1;FQcockt2</t>
+  </si>
+  <si>
+    <t>FQcockt1*FQcockt2</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Cocktails?</t>
+  </si>
+  <si>
+    <t>FQpizza1;FQpizza2;FQchips1;FQchips2</t>
+  </si>
+  <si>
+    <t>(FQpizza1*FQpizza2)+(FQchips1*FQchips2)</t>
+  </si>
+  <si>
+    <t>Wie oft und wieviel Pizza?
+Wie oft und wieviel Kartoffelchips?</t>
+  </si>
+  <si>
+    <t>__BLANK__</t>
+  </si>
+  <si>
+    <t>paste</t>
+  </si>
+  <si>
+    <t>identical</t>
+  </si>
+  <si>
+    <t>1 (FFQ)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -921,13 +1283,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -942,11 +1343,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1287,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="C93" workbookViewId="0">
+      <selection activeCell="I121" sqref="I121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,6 +2686,24 @@
       <c r="D36" t="s">
         <v>13</v>
       </c>
+      <c r="F36" t="s">
+        <v>293</v>
+      </c>
+      <c r="G36" t="s">
+        <v>256</v>
+      </c>
+      <c r="H36" t="s">
+        <v>294</v>
+      </c>
+      <c r="I36" t="s">
+        <v>295</v>
+      </c>
+      <c r="J36" t="s">
+        <v>254</v>
+      </c>
+      <c r="K36" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -2274,6 +2715,21 @@
       <c r="D37" t="s">
         <v>13</v>
       </c>
+      <c r="F37" t="s">
+        <v>262</v>
+      </c>
+      <c r="G37" t="s">
+        <v>262</v>
+      </c>
+      <c r="H37" t="s">
+        <v>262</v>
+      </c>
+      <c r="J37" t="s">
+        <v>262</v>
+      </c>
+      <c r="K37" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -2285,6 +2741,21 @@
       <c r="D38" t="s">
         <v>13</v>
       </c>
+      <c r="F38" t="s">
+        <v>262</v>
+      </c>
+      <c r="G38" t="s">
+        <v>262</v>
+      </c>
+      <c r="H38" t="s">
+        <v>262</v>
+      </c>
+      <c r="J38" t="s">
+        <v>262</v>
+      </c>
+      <c r="K38" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -2296,6 +2767,24 @@
       <c r="D39" t="s">
         <v>13</v>
       </c>
+      <c r="F39" t="s">
+        <v>296</v>
+      </c>
+      <c r="G39" t="s">
+        <v>256</v>
+      </c>
+      <c r="H39" t="s">
+        <v>297</v>
+      </c>
+      <c r="I39" t="s">
+        <v>298</v>
+      </c>
+      <c r="J39" t="s">
+        <v>254</v>
+      </c>
+      <c r="K39" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
@@ -2307,6 +2796,24 @@
       <c r="D40" t="s">
         <v>13</v>
       </c>
+      <c r="F40" t="s">
+        <v>299</v>
+      </c>
+      <c r="G40" t="s">
+        <v>256</v>
+      </c>
+      <c r="H40" t="s">
+        <v>300</v>
+      </c>
+      <c r="I40" t="s">
+        <v>301</v>
+      </c>
+      <c r="J40" t="s">
+        <v>254</v>
+      </c>
+      <c r="K40" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
@@ -2318,6 +2825,21 @@
       <c r="D41" t="s">
         <v>13</v>
       </c>
+      <c r="F41" t="s">
+        <v>262</v>
+      </c>
+      <c r="G41" t="s">
+        <v>262</v>
+      </c>
+      <c r="H41" t="s">
+        <v>262</v>
+      </c>
+      <c r="J41" t="s">
+        <v>262</v>
+      </c>
+      <c r="K41" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
@@ -2329,8 +2851,23 @@
       <c r="D42" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>262</v>
+      </c>
+      <c r="G42" t="s">
+        <v>262</v>
+      </c>
+      <c r="H42" t="s">
+        <v>262</v>
+      </c>
+      <c r="J42" t="s">
+        <v>262</v>
+      </c>
+      <c r="K42" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>94</v>
       </c>
@@ -2339,6 +2876,24 @@
       </c>
       <c r="D43" t="s">
         <v>13</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -2351,6 +2906,21 @@
       <c r="D44" t="s">
         <v>13</v>
       </c>
+      <c r="F44" t="s">
+        <v>262</v>
+      </c>
+      <c r="G44" t="s">
+        <v>262</v>
+      </c>
+      <c r="H44" t="s">
+        <v>262</v>
+      </c>
+      <c r="J44" t="s">
+        <v>262</v>
+      </c>
+      <c r="K44" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -2362,6 +2932,21 @@
       <c r="D45" t="s">
         <v>13</v>
       </c>
+      <c r="F45" t="s">
+        <v>262</v>
+      </c>
+      <c r="G45" t="s">
+        <v>262</v>
+      </c>
+      <c r="H45" t="s">
+        <v>262</v>
+      </c>
+      <c r="J45" t="s">
+        <v>262</v>
+      </c>
+      <c r="K45" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -2373,6 +2958,21 @@
       <c r="D46" t="s">
         <v>13</v>
       </c>
+      <c r="F46" t="s">
+        <v>262</v>
+      </c>
+      <c r="G46" t="s">
+        <v>262</v>
+      </c>
+      <c r="H46" t="s">
+        <v>262</v>
+      </c>
+      <c r="J46" t="s">
+        <v>262</v>
+      </c>
+      <c r="K46" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
@@ -2384,6 +2984,21 @@
       <c r="D47" t="s">
         <v>13</v>
       </c>
+      <c r="F47" t="s">
+        <v>262</v>
+      </c>
+      <c r="G47" t="s">
+        <v>262</v>
+      </c>
+      <c r="H47" t="s">
+        <v>262</v>
+      </c>
+      <c r="J47" t="s">
+        <v>262</v>
+      </c>
+      <c r="K47" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
@@ -2395,8 +3010,23 @@
       <c r="D48" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>262</v>
+      </c>
+      <c r="G48" t="s">
+        <v>262</v>
+      </c>
+      <c r="H48" t="s">
+        <v>262</v>
+      </c>
+      <c r="J48" t="s">
+        <v>262</v>
+      </c>
+      <c r="K48" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>106</v>
       </c>
@@ -2406,8 +3036,23 @@
       <c r="D49" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>262</v>
+      </c>
+      <c r="G49" t="s">
+        <v>262</v>
+      </c>
+      <c r="H49" t="s">
+        <v>262</v>
+      </c>
+      <c r="J49" t="s">
+        <v>262</v>
+      </c>
+      <c r="K49" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>108</v>
       </c>
@@ -2417,8 +3062,26 @@
       <c r="D50" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F50" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>110</v>
       </c>
@@ -2428,8 +3091,23 @@
       <c r="D51" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>262</v>
+      </c>
+      <c r="G51" t="s">
+        <v>262</v>
+      </c>
+      <c r="H51" t="s">
+        <v>262</v>
+      </c>
+      <c r="J51" t="s">
+        <v>262</v>
+      </c>
+      <c r="K51" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>112</v>
       </c>
@@ -2439,8 +3117,23 @@
       <c r="D52" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>262</v>
+      </c>
+      <c r="G52" t="s">
+        <v>262</v>
+      </c>
+      <c r="H52" t="s">
+        <v>262</v>
+      </c>
+      <c r="J52" t="s">
+        <v>262</v>
+      </c>
+      <c r="K52" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>114</v>
       </c>
@@ -2450,8 +3143,23 @@
       <c r="D53" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>262</v>
+      </c>
+      <c r="G53" t="s">
+        <v>262</v>
+      </c>
+      <c r="H53" t="s">
+        <v>262</v>
+      </c>
+      <c r="J53" t="s">
+        <v>262</v>
+      </c>
+      <c r="K53" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>116</v>
       </c>
@@ -2461,8 +3169,23 @@
       <c r="D54" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>262</v>
+      </c>
+      <c r="G54" t="s">
+        <v>262</v>
+      </c>
+      <c r="H54" t="s">
+        <v>262</v>
+      </c>
+      <c r="J54" t="s">
+        <v>262</v>
+      </c>
+      <c r="K54" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>118</v>
       </c>
@@ -2472,8 +3195,23 @@
       <c r="D55" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>262</v>
+      </c>
+      <c r="G55" t="s">
+        <v>262</v>
+      </c>
+      <c r="H55" t="s">
+        <v>262</v>
+      </c>
+      <c r="J55" t="s">
+        <v>262</v>
+      </c>
+      <c r="K55" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>120</v>
       </c>
@@ -2483,8 +3221,23 @@
       <c r="D56" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>262</v>
+      </c>
+      <c r="G56" t="s">
+        <v>262</v>
+      </c>
+      <c r="H56" t="s">
+        <v>262</v>
+      </c>
+      <c r="J56" t="s">
+        <v>262</v>
+      </c>
+      <c r="K56" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>122</v>
       </c>
@@ -2494,8 +3247,23 @@
       <c r="D57" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>262</v>
+      </c>
+      <c r="G57" t="s">
+        <v>262</v>
+      </c>
+      <c r="H57" t="s">
+        <v>262</v>
+      </c>
+      <c r="J57" t="s">
+        <v>262</v>
+      </c>
+      <c r="K57" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" ht="165" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>124</v>
       </c>
@@ -2505,8 +3273,26 @@
       <c r="D58" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F58" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>126</v>
       </c>
@@ -2516,8 +3302,23 @@
       <c r="D59" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>262</v>
+      </c>
+      <c r="G59" t="s">
+        <v>262</v>
+      </c>
+      <c r="H59" t="s">
+        <v>262</v>
+      </c>
+      <c r="J59" t="s">
+        <v>262</v>
+      </c>
+      <c r="K59" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>128</v>
       </c>
@@ -2527,8 +3328,23 @@
       <c r="D60" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>262</v>
+      </c>
+      <c r="G60" t="s">
+        <v>262</v>
+      </c>
+      <c r="H60" t="s">
+        <v>262</v>
+      </c>
+      <c r="J60" t="s">
+        <v>262</v>
+      </c>
+      <c r="K60" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>130</v>
       </c>
@@ -2538,8 +3354,26 @@
       <c r="D61" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F61" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K61" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>132</v>
       </c>
@@ -2549,8 +3383,23 @@
       <c r="D62" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>262</v>
+      </c>
+      <c r="G62" t="s">
+        <v>262</v>
+      </c>
+      <c r="H62" t="s">
+        <v>262</v>
+      </c>
+      <c r="J62" t="s">
+        <v>262</v>
+      </c>
+      <c r="K62" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>134</v>
       </c>
@@ -2560,8 +3409,23 @@
       <c r="D63" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>262</v>
+      </c>
+      <c r="G63" t="s">
+        <v>262</v>
+      </c>
+      <c r="H63" t="s">
+        <v>262</v>
+      </c>
+      <c r="J63" t="s">
+        <v>262</v>
+      </c>
+      <c r="K63" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>136</v>
       </c>
@@ -2571,8 +3435,26 @@
       <c r="D64" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>314</v>
+      </c>
+      <c r="G64" t="s">
+        <v>256</v>
+      </c>
+      <c r="H64" t="s">
+        <v>315</v>
+      </c>
+      <c r="I64" t="s">
+        <v>316</v>
+      </c>
+      <c r="J64" t="s">
+        <v>317</v>
+      </c>
+      <c r="K64" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>138</v>
       </c>
@@ -2582,8 +3464,23 @@
       <c r="D65" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>262</v>
+      </c>
+      <c r="G65" t="s">
+        <v>262</v>
+      </c>
+      <c r="H65" t="s">
+        <v>262</v>
+      </c>
+      <c r="J65" t="s">
+        <v>262</v>
+      </c>
+      <c r="K65" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>140</v>
       </c>
@@ -2593,8 +3490,26 @@
       <c r="D66" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F66" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>142</v>
       </c>
@@ -2604,8 +3519,23 @@
       <c r="D67" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>262</v>
+      </c>
+      <c r="G67" t="s">
+        <v>262</v>
+      </c>
+      <c r="H67" t="s">
+        <v>262</v>
+      </c>
+      <c r="J67" t="s">
+        <v>262</v>
+      </c>
+      <c r="K67" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>144</v>
       </c>
@@ -2615,8 +3545,23 @@
       <c r="D68" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>262</v>
+      </c>
+      <c r="G68" t="s">
+        <v>262</v>
+      </c>
+      <c r="H68" t="s">
+        <v>262</v>
+      </c>
+      <c r="J68" t="s">
+        <v>262</v>
+      </c>
+      <c r="K68" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>146</v>
       </c>
@@ -2626,8 +3571,23 @@
       <c r="D69" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>262</v>
+      </c>
+      <c r="G69" t="s">
+        <v>262</v>
+      </c>
+      <c r="H69" t="s">
+        <v>262</v>
+      </c>
+      <c r="J69" t="s">
+        <v>262</v>
+      </c>
+      <c r="K69" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>148</v>
       </c>
@@ -2637,8 +3597,23 @@
       <c r="D70" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>262</v>
+      </c>
+      <c r="G70" t="s">
+        <v>262</v>
+      </c>
+      <c r="H70" t="s">
+        <v>262</v>
+      </c>
+      <c r="J70" t="s">
+        <v>262</v>
+      </c>
+      <c r="K70" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>150</v>
       </c>
@@ -2648,8 +3623,23 @@
       <c r="D71" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>262</v>
+      </c>
+      <c r="G71" t="s">
+        <v>262</v>
+      </c>
+      <c r="H71" t="s">
+        <v>262</v>
+      </c>
+      <c r="J71" t="s">
+        <v>262</v>
+      </c>
+      <c r="K71" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>152</v>
       </c>
@@ -2659,8 +3649,23 @@
       <c r="D72" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>262</v>
+      </c>
+      <c r="G72" t="s">
+        <v>262</v>
+      </c>
+      <c r="H72" t="s">
+        <v>262</v>
+      </c>
+      <c r="J72" t="s">
+        <v>262</v>
+      </c>
+      <c r="K72" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>154</v>
       </c>
@@ -2670,8 +3675,23 @@
       <c r="D73" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>262</v>
+      </c>
+      <c r="G73" t="s">
+        <v>262</v>
+      </c>
+      <c r="H73" t="s">
+        <v>262</v>
+      </c>
+      <c r="J73" t="s">
+        <v>262</v>
+      </c>
+      <c r="K73" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>156</v>
       </c>
@@ -2681,8 +3701,26 @@
       <c r="D74" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>321</v>
+      </c>
+      <c r="G74" t="s">
+        <v>256</v>
+      </c>
+      <c r="H74" t="s">
+        <v>328</v>
+      </c>
+      <c r="I74" t="s">
+        <v>322</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>158</v>
       </c>
@@ -2692,8 +3730,26 @@
       <c r="D75" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>323</v>
+      </c>
+      <c r="G75" t="s">
+        <v>256</v>
+      </c>
+      <c r="H75" t="s">
+        <v>327</v>
+      </c>
+      <c r="I75" t="s">
+        <v>324</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>160</v>
       </c>
@@ -2703,8 +3759,26 @@
       <c r="D76" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>325</v>
+      </c>
+      <c r="G76" t="s">
+        <v>256</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I76" t="s">
+        <v>332</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>162</v>
       </c>
@@ -2714,8 +3788,23 @@
       <c r="D77" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>262</v>
+      </c>
+      <c r="G77" t="s">
+        <v>262</v>
+      </c>
+      <c r="H77" t="s">
+        <v>262</v>
+      </c>
+      <c r="J77" t="s">
+        <v>262</v>
+      </c>
+      <c r="K77" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>164</v>
       </c>
@@ -2725,8 +3814,26 @@
       <c r="D78" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>329</v>
+      </c>
+      <c r="G78" t="s">
+        <v>256</v>
+      </c>
+      <c r="H78" t="s">
+        <v>330</v>
+      </c>
+      <c r="I78" t="s">
+        <v>331</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>166</v>
       </c>
@@ -2736,8 +3843,23 @@
       <c r="D79" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>262</v>
+      </c>
+      <c r="G79" t="s">
+        <v>262</v>
+      </c>
+      <c r="H79" t="s">
+        <v>262</v>
+      </c>
+      <c r="J79" t="s">
+        <v>262</v>
+      </c>
+      <c r="K79" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>168</v>
       </c>
@@ -2747,8 +3869,23 @@
       <c r="D80" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>262</v>
+      </c>
+      <c r="G80" t="s">
+        <v>262</v>
+      </c>
+      <c r="H80" t="s">
+        <v>262</v>
+      </c>
+      <c r="J80" t="s">
+        <v>262</v>
+      </c>
+      <c r="K80" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>170</v>
       </c>
@@ -2758,8 +3895,23 @@
       <c r="D81" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>262</v>
+      </c>
+      <c r="G81" t="s">
+        <v>262</v>
+      </c>
+      <c r="H81" t="s">
+        <v>262</v>
+      </c>
+      <c r="J81" t="s">
+        <v>262</v>
+      </c>
+      <c r="K81" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>172</v>
       </c>
@@ -2769,8 +3921,26 @@
       <c r="D82" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>333</v>
+      </c>
+      <c r="G82" t="s">
+        <v>256</v>
+      </c>
+      <c r="H82" t="s">
+        <v>334</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>174</v>
       </c>
@@ -2780,8 +3950,23 @@
       <c r="D83" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>262</v>
+      </c>
+      <c r="G83" t="s">
+        <v>262</v>
+      </c>
+      <c r="H83" t="s">
+        <v>262</v>
+      </c>
+      <c r="J83" t="s">
+        <v>262</v>
+      </c>
+      <c r="K83" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>176</v>
       </c>
@@ -2791,8 +3976,23 @@
       <c r="D84" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>262</v>
+      </c>
+      <c r="G84" t="s">
+        <v>262</v>
+      </c>
+      <c r="H84" t="s">
+        <v>262</v>
+      </c>
+      <c r="J84" t="s">
+        <v>262</v>
+      </c>
+      <c r="K84" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>178</v>
       </c>
@@ -2802,8 +4002,23 @@
       <c r="D85" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>262</v>
+      </c>
+      <c r="G85" t="s">
+        <v>262</v>
+      </c>
+      <c r="H85" t="s">
+        <v>262</v>
+      </c>
+      <c r="J85" t="s">
+        <v>262</v>
+      </c>
+      <c r="K85" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" ht="180" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>180</v>
       </c>
@@ -2813,8 +4028,26 @@
       <c r="D86" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F86" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>182</v>
       </c>
@@ -2824,8 +4057,26 @@
       <c r="D87" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>339</v>
+      </c>
+      <c r="G87" t="s">
+        <v>256</v>
+      </c>
+      <c r="H87" t="s">
+        <v>340</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>184</v>
       </c>
@@ -2835,8 +4086,23 @@
       <c r="D88" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>262</v>
+      </c>
+      <c r="G88" t="s">
+        <v>262</v>
+      </c>
+      <c r="H88" t="s">
+        <v>262</v>
+      </c>
+      <c r="J88" t="s">
+        <v>262</v>
+      </c>
+      <c r="K88" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>186</v>
       </c>
@@ -2846,8 +4112,26 @@
       <c r="D89" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F89" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>188</v>
       </c>
@@ -2857,8 +4141,26 @@
       <c r="D90" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F90" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>190</v>
       </c>
@@ -2868,8 +4170,26 @@
       <c r="D91" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F91" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>192</v>
       </c>
@@ -2879,8 +4199,23 @@
       <c r="D92" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>262</v>
+      </c>
+      <c r="G92" t="s">
+        <v>262</v>
+      </c>
+      <c r="H92" t="s">
+        <v>262</v>
+      </c>
+      <c r="J92" t="s">
+        <v>262</v>
+      </c>
+      <c r="K92" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>194</v>
       </c>
@@ -2890,8 +4225,26 @@
       <c r="D93" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>351</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="H93" t="s">
+        <v>352</v>
+      </c>
+      <c r="I93" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="J93" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="K93" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>196</v>
       </c>
@@ -2901,8 +4254,23 @@
       <c r="D94" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
+        <v>262</v>
+      </c>
+      <c r="G94" t="s">
+        <v>262</v>
+      </c>
+      <c r="H94" t="s">
+        <v>262</v>
+      </c>
+      <c r="J94" t="s">
+        <v>262</v>
+      </c>
+      <c r="K94" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>198</v>
       </c>
@@ -2912,8 +4280,26 @@
       <c r="D95" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
+        <v>354</v>
+      </c>
+      <c r="G95" t="s">
+        <v>256</v>
+      </c>
+      <c r="H95" t="s">
+        <v>355</v>
+      </c>
+      <c r="I95" t="s">
+        <v>356</v>
+      </c>
+      <c r="J95" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>200</v>
       </c>
@@ -2923,8 +4309,23 @@
       <c r="D96" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F96" t="s">
+        <v>262</v>
+      </c>
+      <c r="G96" t="s">
+        <v>262</v>
+      </c>
+      <c r="H96" t="s">
+        <v>262</v>
+      </c>
+      <c r="J96" t="s">
+        <v>262</v>
+      </c>
+      <c r="K96" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>202</v>
       </c>
@@ -2934,8 +4335,26 @@
       <c r="D97" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F97" t="s">
+        <v>357</v>
+      </c>
+      <c r="G97" t="s">
+        <v>256</v>
+      </c>
+      <c r="H97" t="s">
+        <v>358</v>
+      </c>
+      <c r="I97" t="s">
+        <v>359</v>
+      </c>
+      <c r="J97" t="s">
+        <v>254</v>
+      </c>
+      <c r="K97" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>204</v>
       </c>
@@ -2945,8 +4364,26 @@
       <c r="D98" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>360</v>
+      </c>
+      <c r="G98" t="s">
+        <v>256</v>
+      </c>
+      <c r="H98" t="s">
+        <v>361</v>
+      </c>
+      <c r="I98" t="s">
+        <v>362</v>
+      </c>
+      <c r="J98" t="s">
+        <v>254</v>
+      </c>
+      <c r="K98" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>206</v>
       </c>
@@ -2956,8 +4393,23 @@
       <c r="D99" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>262</v>
+      </c>
+      <c r="G99" t="s">
+        <v>262</v>
+      </c>
+      <c r="H99" t="s">
+        <v>262</v>
+      </c>
+      <c r="J99" t="s">
+        <v>262</v>
+      </c>
+      <c r="K99" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>208</v>
       </c>
@@ -2967,8 +4419,23 @@
       <c r="D100" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>262</v>
+      </c>
+      <c r="G100" t="s">
+        <v>262</v>
+      </c>
+      <c r="H100" t="s">
+        <v>262</v>
+      </c>
+      <c r="J100" t="s">
+        <v>262</v>
+      </c>
+      <c r="K100" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>210</v>
       </c>
@@ -2978,8 +4445,26 @@
       <c r="D101" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F101" t="s">
+        <v>363</v>
+      </c>
+      <c r="G101" t="s">
+        <v>256</v>
+      </c>
+      <c r="H101" t="s">
+        <v>364</v>
+      </c>
+      <c r="I101" t="s">
+        <v>365</v>
+      </c>
+      <c r="J101" t="s">
+        <v>254</v>
+      </c>
+      <c r="K101" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>212</v>
       </c>
@@ -2989,8 +4474,23 @@
       <c r="D102" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F102" t="s">
+        <v>262</v>
+      </c>
+      <c r="G102" t="s">
+        <v>262</v>
+      </c>
+      <c r="H102" t="s">
+        <v>262</v>
+      </c>
+      <c r="J102" t="s">
+        <v>262</v>
+      </c>
+      <c r="K102" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>214</v>
       </c>
@@ -3000,8 +4500,23 @@
       <c r="D103" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F103" t="s">
+        <v>262</v>
+      </c>
+      <c r="G103" t="s">
+        <v>262</v>
+      </c>
+      <c r="H103" t="s">
+        <v>262</v>
+      </c>
+      <c r="J103" t="s">
+        <v>262</v>
+      </c>
+      <c r="K103" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>216</v>
       </c>
@@ -3011,8 +4526,23 @@
       <c r="D104" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F104" t="s">
+        <v>262</v>
+      </c>
+      <c r="G104" t="s">
+        <v>262</v>
+      </c>
+      <c r="H104" t="s">
+        <v>262</v>
+      </c>
+      <c r="J104" t="s">
+        <v>262</v>
+      </c>
+      <c r="K104" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>218</v>
       </c>
@@ -3022,8 +4552,23 @@
       <c r="D105" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F105" t="s">
+        <v>262</v>
+      </c>
+      <c r="G105" t="s">
+        <v>262</v>
+      </c>
+      <c r="H105" t="s">
+        <v>262</v>
+      </c>
+      <c r="J105" t="s">
+        <v>262</v>
+      </c>
+      <c r="K105" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>220</v>
       </c>
@@ -3033,8 +4578,23 @@
       <c r="D106" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
+        <v>262</v>
+      </c>
+      <c r="G106" t="s">
+        <v>262</v>
+      </c>
+      <c r="H106" t="s">
+        <v>262</v>
+      </c>
+      <c r="J106" t="s">
+        <v>262</v>
+      </c>
+      <c r="K106" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>222</v>
       </c>
@@ -3044,8 +4604,23 @@
       <c r="D107" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>262</v>
+      </c>
+      <c r="G107" t="s">
+        <v>262</v>
+      </c>
+      <c r="H107" t="s">
+        <v>262</v>
+      </c>
+      <c r="J107" t="s">
+        <v>262</v>
+      </c>
+      <c r="K107" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>224</v>
       </c>
@@ -3055,8 +4630,23 @@
       <c r="D108" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F108" t="s">
+        <v>262</v>
+      </c>
+      <c r="G108" t="s">
+        <v>262</v>
+      </c>
+      <c r="H108" t="s">
+        <v>262</v>
+      </c>
+      <c r="J108" t="s">
+        <v>262</v>
+      </c>
+      <c r="K108" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>226</v>
       </c>
@@ -3066,8 +4656,23 @@
       <c r="D109" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
+        <v>262</v>
+      </c>
+      <c r="G109" t="s">
+        <v>262</v>
+      </c>
+      <c r="H109" t="s">
+        <v>262</v>
+      </c>
+      <c r="J109" t="s">
+        <v>262</v>
+      </c>
+      <c r="K109" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>228</v>
       </c>
@@ -3077,8 +4682,23 @@
       <c r="D110" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F110" t="s">
+        <v>262</v>
+      </c>
+      <c r="G110" t="s">
+        <v>262</v>
+      </c>
+      <c r="H110" t="s">
+        <v>262</v>
+      </c>
+      <c r="J110" t="s">
+        <v>262</v>
+      </c>
+      <c r="K110" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>230</v>
       </c>
@@ -3088,8 +4708,23 @@
       <c r="D111" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F111" t="s">
+        <v>262</v>
+      </c>
+      <c r="G111" t="s">
+        <v>262</v>
+      </c>
+      <c r="H111" t="s">
+        <v>262</v>
+      </c>
+      <c r="J111" t="s">
+        <v>262</v>
+      </c>
+      <c r="K111" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>232</v>
       </c>
@@ -3099,8 +4734,23 @@
       <c r="D112" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F112" t="s">
+        <v>262</v>
+      </c>
+      <c r="G112" t="s">
+        <v>262</v>
+      </c>
+      <c r="H112" t="s">
+        <v>262</v>
+      </c>
+      <c r="J112" t="s">
+        <v>262</v>
+      </c>
+      <c r="K112" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>234</v>
       </c>
@@ -3110,8 +4760,23 @@
       <c r="D113" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F113" t="s">
+        <v>262</v>
+      </c>
+      <c r="G113" t="s">
+        <v>262</v>
+      </c>
+      <c r="H113" t="s">
+        <v>262</v>
+      </c>
+      <c r="J113" t="s">
+        <v>262</v>
+      </c>
+      <c r="K113" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>236</v>
       </c>
@@ -3121,8 +4786,23 @@
       <c r="D114" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F114" t="s">
+        <v>262</v>
+      </c>
+      <c r="G114" t="s">
+        <v>262</v>
+      </c>
+      <c r="H114" t="s">
+        <v>262</v>
+      </c>
+      <c r="J114" t="s">
+        <v>262</v>
+      </c>
+      <c r="K114" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>238</v>
       </c>
@@ -3132,8 +4812,23 @@
       <c r="D115" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F115" t="s">
+        <v>262</v>
+      </c>
+      <c r="G115" t="s">
+        <v>262</v>
+      </c>
+      <c r="H115" t="s">
+        <v>262</v>
+      </c>
+      <c r="J115" t="s">
+        <v>262</v>
+      </c>
+      <c r="K115" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>240</v>
       </c>
@@ -3143,8 +4838,23 @@
       <c r="D116" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F116" t="s">
+        <v>262</v>
+      </c>
+      <c r="G116" t="s">
+        <v>262</v>
+      </c>
+      <c r="H116" t="s">
+        <v>262</v>
+      </c>
+      <c r="J116" t="s">
+        <v>262</v>
+      </c>
+      <c r="K116" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>242</v>
       </c>
@@ -3154,8 +4864,23 @@
       <c r="D117" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F117" t="s">
+        <v>262</v>
+      </c>
+      <c r="G117" t="s">
+        <v>262</v>
+      </c>
+      <c r="H117" t="s">
+        <v>262</v>
+      </c>
+      <c r="J117" t="s">
+        <v>262</v>
+      </c>
+      <c r="K117" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>244</v>
       </c>
@@ -3165,8 +4890,23 @@
       <c r="D118" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F118" t="s">
+        <v>262</v>
+      </c>
+      <c r="G118" t="s">
+        <v>262</v>
+      </c>
+      <c r="H118" t="s">
+        <v>262</v>
+      </c>
+      <c r="J118" t="s">
+        <v>262</v>
+      </c>
+      <c r="K118" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="119" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>246</v>
       </c>
@@ -3176,8 +4916,26 @@
       <c r="D119" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F119" t="s">
+        <v>366</v>
+      </c>
+      <c r="G119" t="s">
+        <v>256</v>
+      </c>
+      <c r="H119" t="s">
+        <v>367</v>
+      </c>
+      <c r="I119" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="J119" t="s">
+        <v>254</v>
+      </c>
+      <c r="K119" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>248</v>
       </c>
@@ -3187,8 +4945,23 @@
       <c r="D120" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F120" t="s">
+        <v>262</v>
+      </c>
+      <c r="G120" t="s">
+        <v>262</v>
+      </c>
+      <c r="H120" t="s">
+        <v>262</v>
+      </c>
+      <c r="J120" t="s">
+        <v>262</v>
+      </c>
+      <c r="K120" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>250</v>
       </c>
@@ -3197,6 +4970,24 @@
       </c>
       <c r="D121" t="s">
         <v>252</v>
+      </c>
+      <c r="F121" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G121" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="H121" s="11">
+        <v>1</v>
+      </c>
+      <c r="I121" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="J121" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="K121" s="13" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added an additional comment to DIETARY_ASSESS_INSTR
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_DEGS1_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_DEGS1_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0B30EB3-09F9-439F-B114-5D0E84D35CF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C8F179-B738-421D-8176-09178BFC4143}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -326,6 +315,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Wie oft und  wieviel Quark, Joghurt oder Dickmilch?
@@ -336,6 +326,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Was machen wir mit FQquark3 (Anteil fettarmer Quark, Joghurt, Dickmilch)?</t>
@@ -359,6 +350,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Wie oft und wieviel Frischkäse?
@@ -369,6 +361,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Was machen wir mit FQfkaes3 (Anteil fettarmer Frischkäse)?</t>
@@ -392,6 +385,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Wie oft und wieviel Käse (Weich-, Schnitt- oder Hartkäse)?
@@ -402,6 +396,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Was machen wir mit FQkaes3 (Anteil fettarmer Käse)?</t>
@@ -551,6 +546,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Wie oft und wieviel Fleisch (ohne Geflügel, ohne Wurst) 
@@ -561,6 +557,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Was machen wir mit FQfleisch3 (Wie oft paniertes Fleisch)?</t>
@@ -620,6 +617,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Wie oft und wieviel Geflügel?
@@ -630,6 +628,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Was machen wir mit FGhuhn3 (Anteil paniertes o frittiertes Geflügel)?</t>
@@ -1350,17 +1349,17 @@
     <t>paste</t>
   </si>
   <si>
-    <t>1 (FFQ)</t>
-  </si>
-  <si>
     <t>identical</t>
+  </si>
+  <si>
+    <t>1 (FFQ), but asks only about the last 4 weeks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1372,6 +1371,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1413,19 +1413,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1828,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="H119" sqref="H119"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="K135" sqref="K135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5471,13 +5459,13 @@
         <v>1</v>
       </c>
       <c r="I121" s="10" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="J121" s="11" t="s">
         <v>23</v>
       </c>
       <c r="K121" s="11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -5487,6 +5475,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -5496,15 +5493,6 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5749,26 +5737,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C1076D-2C61-4BAC-A503-5A4B20CD35B7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70A53FE4-D237-4764-9B07-7D2AFF4EC446}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70A53FE4-D237-4764-9B07-7D2AFF4EC446}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C1076D-2C61-4BAC-A503-5A4B20CD35B7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>